<commit_message>
login and zone page commited
</commit_message>
<xml_diff>
--- a/TT231DemoScreenDetail.xlsx
+++ b/TT231DemoScreenDetail.xlsx
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="119">
   <si>
     <t>Notes</t>
   </si>
@@ -99,10 +99,6 @@
   </si>
   <si>
     <t>Column1</t>
-  </si>
-  <si>
-    <t>Screen Description
-Start</t>
   </si>
   <si>
     <t>Login Screen</t>
@@ -419,6 +415,36 @@
   </si>
   <si>
     <t>Create key screens using a normal white background theme</t>
+  </si>
+  <si>
+    <t>Screen Description</t>
+  </si>
+  <si>
+    <t>3.1.4 Incident Record (IR) workflow (8)</t>
+  </si>
+  <si>
+    <t>Figure 3.33</t>
+  </si>
+  <si>
+    <t>Add Equipment to Plan</t>
+  </si>
+  <si>
+    <t>Menu to add a new plan</t>
+  </si>
+  <si>
+    <t>Figure 3.34</t>
+  </si>
+  <si>
+    <t>Multi Select VMS Plans</t>
+  </si>
+  <si>
+    <t>3.1.4 Incident Record (IR) workflow (9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To select mulitple VMS </t>
+  </si>
+  <si>
+    <t>Todo Page 40</t>
   </si>
 </sst>
 </file>
@@ -568,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -589,6 +615,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,7 +752,7 @@
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -788,6 +820,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="18" fillId="4" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -810,45 +845,6 @@
     <cellStyle name="Title" xfId="9" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Century Gothic"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Century Gothic"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="3" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Century Gothic"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -886,6 +882,7 @@
         <name val="Century Gothic"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="3" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -898,6 +895,20 @@
         <name val="Century Gothic"/>
         <scheme val="minor"/>
       </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Century Gothic"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -941,6 +952,30 @@
           <color theme="9"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Century Gothic"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Century Gothic"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1040,17 +1075,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ProjectTracker3" displayName="ProjectTracker3" ref="A3:H27" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="10" headerRowCellStyle="Heading 2">
-  <autoFilter ref="A3:H27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ProjectTracker3" displayName="ProjectTracker3" ref="A3:H29" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A3:H29"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Modules" dataDxfId="9" dataCellStyle="Text"/>
-    <tableColumn id="3" name="Screen" dataDxfId="8" dataCellStyle="Text"/>
+    <tableColumn id="1" name="Modules" dataDxfId="7" dataCellStyle="Text"/>
+    <tableColumn id="3" name="Screen" dataDxfId="6" dataCellStyle="Text"/>
     <tableColumn id="2" name="Sub Screens" dataDxfId="5" dataCellStyle="Text"/>
-    <tableColumn id="4" name="Screen Description_x000a_Start" dataDxfId="2" dataCellStyle="Date"/>
-    <tableColumn id="5" name="Reference_x000a_Document" dataDxfId="0" dataCellStyle="Date"/>
-    <tableColumn id="6" name="Figure" dataDxfId="1" dataCellStyle="Date"/>
-    <tableColumn id="12" name="Notes" dataDxfId="4" dataCellStyle="Text"/>
-    <tableColumn id="7" name="Doubt" dataDxfId="3"/>
+    <tableColumn id="4" name="Screen Description" dataDxfId="4" dataCellStyle="Date"/>
+    <tableColumn id="5" name="Reference_x000a_Document" dataDxfId="3" dataCellStyle="Date"/>
+    <tableColumn id="6" name="Figure" dataDxfId="2" dataCellStyle="Date"/>
+    <tableColumn id="12" name="Notes" dataDxfId="1" dataCellStyle="Text"/>
+    <tableColumn id="7" name="Doubt" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Custom Table Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1306,10 +1341,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1327,7 +1362,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -1337,375 +1372,375 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="F7" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>31</v>
-      </c>
       <c r="G9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="G10" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="G11" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>44</v>
-      </c>
       <c r="G13" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="F14" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="F15" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="19" t="s">
-        <v>56</v>
-      </c>
       <c r="G15" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="E16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>59</v>
-      </c>
       <c r="G16" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="16" t="s">
         <v>64</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>65</v>
       </c>
       <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="12"/>
       <c r="E18" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="16"/>
       <c r="H18" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="20"/>
@@ -1713,63 +1748,63 @@
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="E20" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="E21" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>81</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>90</v>
-      </c>
       <c r="F22" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="20"/>
@@ -1777,19 +1812,19 @@
     <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>95</v>
-      </c>
       <c r="D23" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="20"/>
@@ -1797,19 +1832,19 @@
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="20" t="s">
-        <v>100</v>
-      </c>
       <c r="F24" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="20"/>
@@ -1817,52 +1852,90 @@
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>103</v>
-      </c>
       <c r="D25" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="19"/>
+      <c r="B27" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>111</v>
+      </c>
       <c r="G27" s="16"/>
       <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="7">
@@ -1916,12 +1989,12 @@
     </row>
     <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1950,6 +2023,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e39e7e9e36de66d473ce04bb4ab2dbb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19dc5994665da46609c24125788630d8" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -2154,24 +2244,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4875-2E31-4ACC-AEED-0DAFD072C30B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2188,22 +2279,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
map and table format added
</commit_message>
<xml_diff>
--- a/TT231DemoScreenDetail.xlsx
+++ b/TT231DemoScreenDetail.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Screens" sheetId="3" r:id="rId1"/>
     <sheet name="Setup" sheetId="2" r:id="rId2"/>
+    <sheet name="Development Pg Info" sheetId="4" r:id="rId3"/>
+    <sheet name="lati-logi" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc535884" localSheetId="0">Screens!$E$19</definedName>
@@ -87,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="185">
   <si>
     <t>Notes</t>
   </si>
@@ -445,6 +447,204 @@
   </si>
   <si>
     <t>Todo Page 40</t>
+  </si>
+  <si>
+    <t>Screen Info</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>login.html</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>zone selection screen</t>
+  </si>
+  <si>
+    <t>zoneselection1.jsp</t>
+  </si>
+  <si>
+    <t>common control 2 (cc2)</t>
+  </si>
+  <si>
+    <t>ccgridview.jsp</t>
+  </si>
+  <si>
+    <t>doing</t>
+  </si>
+  <si>
+    <t>ccgridmergeinc.jsp</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>2. Remove 'Over' status from the Incident</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>CC2</t>
+  </si>
+  <si>
+    <t>3. Create 5 different chart data and change it accordingly</t>
+  </si>
+  <si>
+    <t>4. Work Order remove "Overdue work" from work order</t>
+  </si>
+  <si>
+    <t>5. Display different incident in each panel</t>
+  </si>
+  <si>
+    <t>BIS</t>
+  </si>
+  <si>
+    <t>BIS Work Station and BIS Desktop</t>
+  </si>
+  <si>
+    <t>follow BIS WorkStation</t>
+  </si>
+  <si>
+    <t>D3Js.com</t>
+  </si>
+  <si>
+    <t>Task todo</t>
+  </si>
+  <si>
+    <t>X -  no of roadwork</t>
+  </si>
+  <si>
+    <t>X - Speed data (50, 100)</t>
+  </si>
+  <si>
+    <t>Y - Kilo meter  (24,25,26)</t>
+  </si>
+  <si>
+    <t>2. Road Work - Bar Chart</t>
+  </si>
+  <si>
+    <t>Y - display major road (Expressway, Aye, CTE etc.,)</t>
+  </si>
+  <si>
+    <t>1. Speed Line graph (line Chart) - both direction</t>
+  </si>
+  <si>
+    <t>1. Create 5 files  with different no. of records and push different files in different timing.</t>
+  </si>
+  <si>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t>1. Confiture arcGIS setup locally</t>
+  </si>
+  <si>
+    <t>2. download all libraries</t>
+  </si>
+  <si>
+    <t>3. deploy it in server</t>
+  </si>
+  <si>
+    <t>4. Use the url to get the functionality</t>
+  </si>
+  <si>
+    <t>5. but u need to call it with url</t>
+  </si>
+  <si>
+    <t>Location MRT</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>file:///C:/GisMap/popupinmap.html</t>
+  </si>
+  <si>
+    <t>use this file to get latitude and longitude info</t>
+  </si>
+  <si>
+    <t>MRT - Redhill</t>
+  </si>
+  <si>
+    <t>MRT -  Outram Park</t>
+  </si>
+  <si>
+    <t>MRT - Queenstown</t>
+  </si>
+  <si>
+    <t>North Buona Vista Road, Singapore</t>
+  </si>
+  <si>
+    <t>MRT-Dover</t>
+  </si>
+  <si>
+    <t>CreateMRTIncident</t>
+  </si>
+  <si>
+    <t>MRT Incident</t>
+  </si>
+  <si>
+    <t>createmrtwin.jsp</t>
+  </si>
+  <si>
+    <t>Main File</t>
+  </si>
+  <si>
+    <t>mrtmap.css</t>
+  </si>
+  <si>
+    <t>css file</t>
+  </si>
+  <si>
+    <t>mrtmap.js</t>
+  </si>
+  <si>
+    <t>js file</t>
+  </si>
+  <si>
+    <t>Incident</t>
+  </si>
+  <si>
+    <t>createirwintbl.jsp</t>
+  </si>
+  <si>
+    <t>table format view - title bar, left panel (Map), right panel (incident detail)</t>
+  </si>
+  <si>
+    <t>image file</t>
+  </si>
+  <si>
+    <t>trainy.png</t>
+  </si>
+  <si>
+    <t>createmrtincwin.jsp</t>
+  </si>
+  <si>
+    <t>Map and MRT line selection</t>
+  </si>
+  <si>
+    <t>mrtinc.css</t>
+  </si>
+  <si>
+    <t>Map CSS file</t>
+  </si>
+  <si>
+    <t>Map JS File</t>
+  </si>
+  <si>
+    <t>Train Image</t>
+  </si>
+  <si>
+    <t>MRT Create incident  left display Menu</t>
   </si>
 </sst>
 </file>
@@ -454,7 +654,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Over/Under flag&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
@@ -593,6 +793,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF323232"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -706,7 +942,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -751,8 +987,11 @@
     <xf numFmtId="3" fontId="8" fillId="2" borderId="6">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -825,8 +1064,32 @@
     <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="16">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="17">
     <cellStyle name="Actual Start" xfId="13"/>
     <cellStyle name="Date" xfId="8"/>
     <cellStyle name="Estimated duration" xfId="15"/>
@@ -836,6 +1099,7 @@
     <cellStyle name="Heading 2" xfId="6" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8"/>
     <cellStyle name="Input" xfId="2" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="7" builtinId="10" customBuiltin="1"/>
@@ -1343,8 +1607,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2022,16 +2286,389 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="24.25" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="61.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>178</v>
+      </c>
+      <c r="E44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="28" customWidth="1"/>
+    <col min="3" max="3" width="31.375" customWidth="1"/>
+    <col min="4" max="4" width="42.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="28">
+        <v>103.839</v>
+      </c>
+      <c r="B2" s="28">
+        <v>1.2809999999999999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="29">
+        <v>103.81699999999999</v>
+      </c>
+      <c r="B3" s="28">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="28">
+        <v>103.806</v>
+      </c>
+      <c r="B4" s="28">
+        <v>1.294</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="28">
+        <v>103.79</v>
+      </c>
+      <c r="B5" s="28">
+        <v>1.3069999999999999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="28">
+        <v>103.77800000000001</v>
+      </c>
+      <c r="B6" s="28">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="C6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="31"/>
+      <c r="B9" s="30"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="31"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="30"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="30"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="../../../../../GisMap/popupinmap.html"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
@@ -2039,7 +2676,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e39e7e9e36de66d473ce04bb4ab2dbb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19dc5994665da46609c24125788630d8" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -2244,15 +2881,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2262,7 +2900,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4875-2E31-4ACC-AEED-0DAFD072C30B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2279,4 +2917,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mrt and Event creation with map and UI part merged
</commit_message>
<xml_diff>
--- a/TT231DemoScreenDetail.xlsx
+++ b/TT231DemoScreenDetail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8670" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8676" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Screens" sheetId="3" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="196">
   <si>
     <t>Notes</t>
   </si>
@@ -479,9 +479,6 @@
     <t>doing</t>
   </si>
   <si>
-    <t>ccgridmergeinc.jsp</t>
-  </si>
-  <si>
     <t>Steps</t>
   </si>
   <si>
@@ -617,34 +614,70 @@
     <t>createirwintbl.jsp</t>
   </si>
   <si>
-    <t>table format view - title bar, left panel (Map), right panel (incident detail)</t>
-  </si>
-  <si>
-    <t>image file</t>
-  </si>
-  <si>
     <t>trainy.png</t>
   </si>
   <si>
-    <t>createmrtincwin.jsp</t>
-  </si>
-  <si>
     <t>Map and MRT line selection</t>
   </si>
   <si>
     <t>mrtinc.css</t>
   </si>
   <si>
-    <t>Map CSS file</t>
-  </si>
-  <si>
-    <t>Map JS File</t>
-  </si>
-  <si>
-    <t>Train Image</t>
-  </si>
-  <si>
     <t>MRT Create incident  left display Menu</t>
+  </si>
+  <si>
+    <t>roadmap.jpg</t>
+  </si>
+  <si>
+    <t>Image file for the mrt selection stations (first page)</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/DemoTrans/createmrtwin.jsp</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>1. MRT breakdown selection page</t>
+  </si>
+  <si>
+    <t>2. draw line on the map mrt breakdowns</t>
+  </si>
+  <si>
+    <t>static map image</t>
+  </si>
+  <si>
+    <t>3. ArcGis base map used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pending Task : </t>
+  </si>
+  <si>
+    <t>Progress bar</t>
+  </si>
+  <si>
+    <t>Graph animation</t>
+  </si>
+  <si>
+    <t>Train image file</t>
+  </si>
+  <si>
+    <t>createventwin.jsp</t>
+  </si>
+  <si>
+    <t>Event creation</t>
+  </si>
+  <si>
+    <t>UI layer CSS code</t>
+  </si>
+  <si>
+    <t>map layer css code</t>
+  </si>
+  <si>
+    <t>eventmap.js</t>
+  </si>
+  <si>
+    <t>Map layer function Java Script file</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1024,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1087,6 +1120,18 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1611,27 +1656,27 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.25" customWidth="1"/>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" customWidth="1"/>
     <col min="4" max="4" width="50.5" style="17" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.375" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="6" max="6" width="16.09765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.3984375" customWidth="1"/>
+    <col min="8" max="8" width="16.3984375" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1657,7 +1702,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +1724,7 @@
       </c>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -1701,7 +1746,7 @@
       </c>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -1725,7 +1770,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -1747,7 +1792,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1769,7 +1814,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -1791,7 +1836,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
@@ -1813,7 +1858,7 @@
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -1835,7 +1880,7 @@
       </c>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1857,7 +1902,7 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="10" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1881,7 +1926,7 @@
       </c>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -1905,7 +1950,7 @@
       </c>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>51</v>
@@ -1927,7 +1972,7 @@
       </c>
       <c r="H15" s="20"/>
     </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>59</v>
@@ -1951,7 +1996,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>59</v>
@@ -1971,7 +2016,7 @@
       </c>
       <c r="H17" s="20"/>
     </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>65</v>
       </c>
@@ -1987,7 +2032,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>68</v>
       </c>
@@ -2009,7 +2054,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>75</v>
@@ -2031,7 +2076,7 @@
       </c>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
         <v>82</v>
@@ -2053,7 +2098,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>86</v>
@@ -2073,7 +2118,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>93</v>
@@ -2093,7 +2138,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>96</v>
@@ -2113,7 +2158,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>101</v>
@@ -2133,7 +2178,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
@@ -2151,7 +2196,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
         <v>112</v>
@@ -2171,7 +2216,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
         <v>115</v>
@@ -2189,7 +2234,7 @@
       <c r="G28" s="16"/>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -2236,41 +2281,41 @@
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.625" customWidth="1"/>
+    <col min="1" max="1" width="66.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
   </sheetData>
@@ -2288,25 +2333,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="24.25" customWidth="1"/>
+    <col min="2" max="2" width="24.19921875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="61.25" customWidth="1"/>
+    <col min="4" max="4" width="37.09765625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="44.59765625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="59.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>119</v>
@@ -2314,14 +2360,17 @@
       <c r="C1" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
@@ -2331,24 +2380,24 @@
       <c r="C2" t="s">
         <v>122</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="33" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>124</v>
       </c>
       <c r="C3" t="s">
         <v>125</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="33" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
@@ -2356,205 +2405,246 @@
       <c r="C4" t="s">
         <v>127</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="E6" s="33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="E7" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="35" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="E25" s="33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" t="s">
-        <v>141</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E23" s="24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="25" t="s">
+      <c r="E31" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="E31" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E32" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E33" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="33" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E34" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" t="s">
         <v>166</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>165</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" s="33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>170</v>
       </c>
-      <c r="E38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
+      <c r="D39" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" s="33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>174</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="E43" s="33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>172</v>
       </c>
-      <c r="E39" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C48" t="s">
+        <v>173</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" t="s">
+        <v>190</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
         <v>176</v>
       </c>
-      <c r="E40" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>173</v>
-      </c>
-      <c r="C43" t="s">
-        <v>174</v>
-      </c>
-      <c r="E43" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
-        <v>180</v>
-      </c>
-      <c r="E45" t="s">
-        <v>184</v>
+      <c r="D52" s="33" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>168</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F37" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2566,29 +2656,29 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="12.09765625" style="28" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="28" customWidth="1"/>
-    <col min="3" max="3" width="31.375" customWidth="1"/>
-    <col min="4" max="4" width="42.75" customWidth="1"/>
+    <col min="3" max="3" width="31.3984375" customWidth="1"/>
+    <col min="4" max="4" width="42.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>157</v>
-      </c>
       <c r="C1" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28">
         <v>103.839</v>
       </c>
@@ -2596,13 +2686,13 @@
         <v>1.2809999999999999</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <v>103.81699999999999</v>
       </c>
@@ -2610,10 +2700,10 @@
         <v>1.2889999999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>103.806</v>
       </c>
@@ -2621,10 +2711,10 @@
         <v>1.294</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>103.79</v>
       </c>
@@ -2632,10 +2722,10 @@
         <v>1.3069999999999999</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>103.77800000000001</v>
       </c>
@@ -2643,20 +2733,20 @@
         <v>1.3120000000000001</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="30"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C12" s="30"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C14" s="30"/>
     </row>
   </sheetData>
@@ -2677,6 +2767,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e39e7e9e36de66d473ce04bb4ab2dbb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19dc5994665da46609c24125788630d8" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -2881,15 +2980,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
   <ds:schemaRefs>
@@ -2901,6 +2991,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4875-2E31-4ACC-AEED-0DAFD072C30B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2917,12 +3015,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
arcgic and basemap and another maven project
</commit_message>
<xml_diff>
--- a/TT231DemoScreenDetail.xlsx
+++ b/TT231DemoScreenDetail.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8676" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8676" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Screens" sheetId="3" r:id="rId1"/>
     <sheet name="Setup" sheetId="2" r:id="rId2"/>
     <sheet name="Development Pg Info" sheetId="4" r:id="rId3"/>
     <sheet name="lati-logi" sheetId="5" r:id="rId4"/>
+    <sheet name="&lt;DIV&gt; notes" sheetId="6" r:id="rId5"/>
+    <sheet name="Graph" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc535884" localSheetId="0">Screens!$E$19</definedName>
@@ -89,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="223">
   <si>
     <t>Notes</t>
   </si>
@@ -599,21 +601,12 @@
     <t>mrtmap.css</t>
   </si>
   <si>
-    <t>css file</t>
-  </si>
-  <si>
     <t>mrtmap.js</t>
   </si>
   <si>
-    <t>js file</t>
-  </si>
-  <si>
     <t>Incident</t>
   </si>
   <si>
-    <t>createirwintbl.jsp</t>
-  </si>
-  <si>
     <t>trainy.png</t>
   </si>
   <si>
@@ -668,16 +661,106 @@
     <t>Event creation</t>
   </si>
   <si>
-    <t>UI layer CSS code</t>
-  </si>
-  <si>
-    <t>map layer css code</t>
-  </si>
-  <si>
     <t>eventmap.js</t>
   </si>
   <si>
     <t>Map layer function Java Script file</t>
+  </si>
+  <si>
+    <t>Step to add "VMS msg inside Div" on map</t>
+  </si>
+  <si>
+    <t>2. create div in css - mrtmap.css</t>
+  </si>
+  <si>
+    <t>3. write js function - eventmap.js</t>
+  </si>
+  <si>
+    <t>4. write vms message in - democontroller.js</t>
+  </si>
+  <si>
+    <t>1. add one row in datapenal column jsp and div tag on the map column- createventwin.jsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. add one row in datapenal column jsp and div tag on the map column- </t>
+  </si>
+  <si>
+    <t>democontroller.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ng-model message </t>
+  </si>
+  <si>
+    <t>(All event related javascrip available to display on the map)</t>
+  </si>
+  <si>
+    <t>map div, vms message div available</t>
+  </si>
+  <si>
+    <t>All UI panel display css available - like button, textarea etc</t>
+  </si>
+  <si>
+    <t>103.859, 1.337   Toa Payoh</t>
+  </si>
+  <si>
+    <t>103.898, 1.372 Hougang</t>
+  </si>
+  <si>
+    <t>103.925, 1.336 Bedok</t>
+  </si>
+  <si>
+    <t>103.957, 1.345 simei</t>
+  </si>
+  <si>
+    <t>103.902, 1.323 Eunos</t>
+  </si>
+  <si>
+    <t>CCTV Camera</t>
+  </si>
+  <si>
+    <t>Serangoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ang Mo Kio</t>
+  </si>
+  <si>
+    <t>103.84, 1.329</t>
+  </si>
+  <si>
+    <t>103.85, 1.327</t>
+  </si>
+  <si>
+    <t>103.846, 1.322</t>
+  </si>
+  <si>
+    <t>103.86, 1.317</t>
+  </si>
+  <si>
+    <t>cctv.png</t>
+  </si>
+  <si>
+    <t>roadwork1.jpg</t>
+  </si>
+  <si>
+    <t>UI layer - side panel display css</t>
+  </si>
+  <si>
+    <t>map layer property css code</t>
+  </si>
+  <si>
+    <t>cctv camera image</t>
+  </si>
+  <si>
+    <t>roadwork image</t>
+  </si>
+  <si>
+    <t>createirwin1.jsp</t>
+  </si>
+  <si>
+    <t>irmap.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change the graph type </t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1107,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1132,6 +1215,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1372,6 +1458,363 @@
         <a:xfrm>
           <a:off x="8420100" y="1076325"/>
           <a:ext cx="2190750" cy="247685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4359018</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>76</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11803380" y="9989820"/>
+          <a:ext cx="4359018" cy="876376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4359018</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2385060" y="175260"/>
+          <a:ext cx="4359018" cy="876376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3292125</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152565</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3703320" y="2804160"/>
+          <a:ext cx="3292125" cy="1905165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>343719</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>30574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3703320" y="1226820"/>
+          <a:ext cx="9449619" cy="1082134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2926334</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3703320" y="5082540"/>
+          <a:ext cx="2926334" cy="1188823"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3627432</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>129674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3733800" y="6819900"/>
+          <a:ext cx="3596952" cy="1546994"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1646063</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>167670</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3703320" y="6484620"/>
+          <a:ext cx="1646063" cy="342930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3589331</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>53390</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3703320" y="8763000"/>
+          <a:ext cx="3589331" cy="579170"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289974</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>137369</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1744980" y="350520"/>
+          <a:ext cx="4778154" cy="2415749"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2333,11 +2776,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2367,7 +2810,7 @@
         <v>129</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2434,17 +2877,17 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="34" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="35" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" s="35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2533,10 +2976,10 @@
         <v>167</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,96 +2990,170 @@
         <v>168</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D41" s="33" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>214</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="E43" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="E42" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="E43" s="33" t="s">
-        <v>179</v>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>215</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" t="s">
+        <v>220</v>
+      </c>
+      <c r="E48" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="C48" t="s">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
+      <c r="C49" t="s">
         <v>173</v>
       </c>
-      <c r="E48" s="33" t="s">
-        <v>175</v>
+      <c r="D49" s="33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
+      <c r="C50" t="s">
+        <v>168</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="24"/>
+      <c r="C51" t="s">
+        <v>221</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="24"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="24"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C55" t="s">
+        <v>187</v>
+      </c>
+      <c r="E55" s="33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>168</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>189</v>
+      </c>
+      <c r="D58" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="E51" s="33" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>176</v>
-      </c>
-      <c r="D52" s="33" t="s">
+      <c r="E58" s="33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>197</v>
+      </c>
+      <c r="E59" s="33" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>168</v>
-      </c>
-      <c r="D53" s="33" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="33" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="33" t="s">
         <v>194</v>
-      </c>
-      <c r="D54" s="33" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2645,15 +3162,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2740,33 +3258,269 @@
       <c r="A9" s="31"/>
       <c r="B9" s="30"/>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="24" t="s">
+        <v>207</v>
+      </c>
+    </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="31" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="C12" s="30"/>
+      <c r="A12" s="28">
+        <v>103.884</v>
+      </c>
+      <c r="B12" s="28">
+        <v>1.3580000000000001</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="28">
+        <v>103.851</v>
+      </c>
+      <c r="B13" s="28">
+        <v>1.373</v>
+      </c>
+      <c r="C13" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>203</v>
+      </c>
       <c r="C14" s="30"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="28">
+        <v>103.839</v>
+      </c>
+      <c r="B18" s="28">
+        <v>1.2809999999999999</v>
+      </c>
+      <c r="C18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>103.81699999999999</v>
+      </c>
+      <c r="B19" s="28">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="28">
+        <v>103.806</v>
+      </c>
+      <c r="B20" s="28">
+        <v>1.294</v>
+      </c>
+      <c r="C20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="28">
+        <v>103.79</v>
+      </c>
+      <c r="B29" s="28">
+        <v>1.3069999999999999</v>
+      </c>
+      <c r="C29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="28">
+        <v>103.77800000000001</v>
+      </c>
+      <c r="B30" s="28">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="C30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>211</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="../../../../../GisMap/popupinmap.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.59765625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="57.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="33" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.8984375" customWidth="1"/>
+    <col min="2" max="2" width="23.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2775,7 +3529,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e39e7e9e36de66d473ce04bb4ab2dbb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19dc5994665da46609c24125788630d8" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -2980,17 +3734,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2998,7 +3750,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4875-2E31-4ACC-AEED-0DAFD072C30B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3015,4 +3767,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Traffic Video and wmts/wms layer
</commit_message>
<xml_diff>
--- a/TT231DemoScreenDetail.xlsx
+++ b/TT231DemoScreenDetail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8676" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8670" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Screens" sheetId="3" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="lati-logi" sheetId="5" r:id="rId4"/>
     <sheet name="&lt;DIV&gt; notes" sheetId="6" r:id="rId5"/>
     <sheet name="Graph" sheetId="7" r:id="rId6"/>
+    <sheet name="GIS" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc535884" localSheetId="0">Screens!$E$19</definedName>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="232">
   <si>
     <t>Notes</t>
   </si>
@@ -761,6 +762,33 @@
   </si>
   <si>
     <t xml:space="preserve">change the graph type </t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSLayer - </t>
+  </si>
+  <si>
+    <t>loadwms2.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMTS Layer – </t>
+  </si>
+  <si>
+    <t>localmapzoom.html</t>
+  </si>
+  <si>
+    <t>Load base map using openmaptile server map and use wmts layer from arcgis api</t>
+  </si>
+  <si>
+    <t>Load VMS img using geoserver on the map using wmslayer form arcgis api</t>
   </si>
 </sst>
 </file>
@@ -770,7 +798,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Over/Under flag&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
@@ -945,6 +973,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1107,7 +1142,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1218,6 +1253,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -2099,27 +2137,27 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" customWidth="1"/>
-    <col min="2" max="2" width="22.59765625" customWidth="1"/>
-    <col min="3" max="3" width="16.8984375" customWidth="1"/>
+    <col min="1" max="1" width="23.25" customWidth="1"/>
+    <col min="2" max="2" width="22.625" customWidth="1"/>
+    <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="4" max="4" width="50.5" style="17" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.09765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.3984375" customWidth="1"/>
-    <col min="8" max="8" width="16.3984375" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.375" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2145,7 +2183,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -2167,7 +2205,7 @@
       </c>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -2189,7 +2227,7 @@
       </c>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -2213,7 +2251,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -2235,7 +2273,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -2257,7 +2295,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -2279,7 +2317,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
@@ -2301,7 +2339,7 @@
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -2323,7 +2361,7 @@
       </c>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -2345,7 +2383,7 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="10" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -2369,7 +2407,7 @@
       </c>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -2393,7 +2431,7 @@
       </c>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>51</v>
@@ -2415,7 +2453,7 @@
       </c>
       <c r="H15" s="20"/>
     </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>59</v>
@@ -2439,7 +2477,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>59</v>
@@ -2459,7 +2497,7 @@
       </c>
       <c r="H17" s="20"/>
     </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>65</v>
       </c>
@@ -2475,7 +2513,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>68</v>
       </c>
@@ -2497,7 +2535,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>75</v>
@@ -2519,7 +2557,7 @@
       </c>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
         <v>82</v>
@@ -2541,7 +2579,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>86</v>
@@ -2561,7 +2599,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>93</v>
@@ -2581,7 +2619,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>96</v>
@@ -2601,7 +2639,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>101</v>
@@ -2621,7 +2659,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
@@ -2639,7 +2677,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
         <v>112</v>
@@ -2659,7 +2697,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
         <v>115</v>
@@ -2677,7 +2715,7 @@
       <c r="G28" s="16"/>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -2724,41 +2762,41 @@
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.59765625" customWidth="1"/>
+    <col min="1" max="1" width="66.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
     </row>
   </sheetData>
@@ -2783,17 +2821,17 @@
       <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="24.19921875" customWidth="1"/>
+    <col min="2" max="2" width="24.25" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="37.09765625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="44.59765625" style="33" customWidth="1"/>
-    <col min="6" max="6" width="59.59765625" customWidth="1"/>
+    <col min="4" max="4" width="37.125" style="33" customWidth="1"/>
+    <col min="5" max="5" width="44.625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="59.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>131</v>
       </c>
@@ -2813,7 +2851,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
@@ -2827,7 +2865,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>124</v>
       </c>
@@ -2838,7 +2876,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>132</v>
       </c>
@@ -2855,47 +2893,47 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E5" s="33" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="E6" s="33" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="E7" s="33" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E8" s="33" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E9" s="34" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E10" s="35" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E11" s="35" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -2909,7 +2947,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>138</v>
       </c>
@@ -2917,27 +2955,27 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E21" s="33" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E23" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E24" s="33" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="E25" s="33" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
         <v>148</v>
       </c>
@@ -2945,27 +2983,27 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E32" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E33" s="33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E34" s="33" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E35" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>165</v>
       </c>
@@ -2982,7 +3020,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>164</v>
       </c>
@@ -2996,7 +3034,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>169</v>
       </c>
@@ -3007,7 +3045,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>171</v>
       </c>
@@ -3015,7 +3053,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>175</v>
       </c>
@@ -3023,7 +3061,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>173</v>
       </c>
@@ -3034,7 +3072,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
         <v>214</v>
       </c>
@@ -3045,7 +3083,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
         <v>215</v>
       </c>
@@ -3053,7 +3091,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>170</v>
       </c>
@@ -3064,7 +3102,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="24"/>
       <c r="C49" t="s">
         <v>173</v>
@@ -3073,7 +3111,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="24"/>
       <c r="C50" t="s">
         <v>168</v>
@@ -3082,7 +3120,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="24"/>
       <c r="C51" t="s">
         <v>221</v>
@@ -3091,13 +3129,13 @@
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="24"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="24"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>38</v>
       </c>
@@ -3108,7 +3146,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
         <v>173</v>
       </c>
@@ -3116,7 +3154,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>168</v>
       </c>
@@ -3127,7 +3165,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>189</v>
       </c>
@@ -3138,7 +3176,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>197</v>
       </c>
@@ -3146,12 +3184,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E60" s="33" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E61" s="33" t="s">
         <v>194</v>
       </c>
@@ -3174,15 +3212,15 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.09765625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="12.125" style="28" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="28" customWidth="1"/>
-    <col min="3" max="3" width="31.3984375" customWidth="1"/>
-    <col min="4" max="4" width="42.69921875" customWidth="1"/>
+    <col min="3" max="3" width="31.375" customWidth="1"/>
+    <col min="4" max="4" width="42.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>155</v>
       </c>
@@ -3196,7 +3234,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>103.839</v>
       </c>
@@ -3210,7 +3248,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>103.81699999999999</v>
       </c>
@@ -3221,7 +3259,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>103.806</v>
       </c>
@@ -3232,7 +3270,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>103.79</v>
       </c>
@@ -3243,7 +3281,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>103.77800000000001</v>
       </c>
@@ -3254,21 +3292,21 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
       <c r="B9" s="30"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" s="24" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
         <v>103.884</v>
       </c>
@@ -3279,7 +3317,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>103.851</v>
       </c>
@@ -3290,28 +3328,28 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
         <v>203</v>
       </c>
       <c r="C14" s="30"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>103.839</v>
       </c>
@@ -3322,7 +3360,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>103.81699999999999</v>
       </c>
@@ -3333,7 +3371,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
         <v>103.806</v>
       </c>
@@ -3344,42 +3382,42 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C24" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="28">
         <v>103.79</v>
       </c>
@@ -3390,7 +3428,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="28">
         <v>103.77800000000001</v>
       </c>
@@ -3401,12 +3439,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>211</v>
       </c>
@@ -3428,63 +3466,63 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.59765625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="57.8984375" customWidth="1"/>
+    <col min="1" max="1" width="48.625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="57.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="33" x14ac:dyDescent="0.3">
       <c r="A30" s="33" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="32" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="32" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="33" x14ac:dyDescent="0.3">
       <c r="A56" s="33" t="s">
         <v>201</v>
       </c>
@@ -3499,17 +3537,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.8984375" customWidth="1"/>
-    <col min="2" max="2" width="23.69921875" customWidth="1"/>
+    <col min="1" max="1" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="23.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -3520,13 +3558,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="71.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3735,17 +3826,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3770,11 +3864,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>